<commit_message>
menuler eklendi. sql bağlantıları sağlandı. öğrenci bilgileri ekranında filtreleme eklendi.
</commit_message>
<xml_diff>
--- a/Kitap1.xlsx
+++ b/Kitap1.xlsx
@@ -5,12 +5,12 @@
   <workbookPr codeName="BuÇalismaKitabi" defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mtshbz\Documents\Projects\C#\databaseProject\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mtshbz\Documents\Projects\C#\databaseProject\databaseProject\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3770E068-2012-45C1-AB3C-5C9D642CE9DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8AF3FDCF-AC1B-41CB-94A8-384CCA6FDA5F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{CD00BCB3-D045-4DCA-ACA0-06FE11EAD6BD}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{CD00BCB3-D045-4DCA-ACA0-06FE11EAD6BD}"/>
   </bookViews>
   <sheets>
     <sheet name="süre" sheetId="6" r:id="rId1"/>
@@ -2887,11 +2887,11 @@
   <sheetPr codeName="Sayfa1"/>
   <dimension ref="A1:C183"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <selection activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="12" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10.5546875" style="1" bestFit="1" customWidth="1"/>
@@ -4560,10 +4560,10 @@
   <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="11.33203125" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="5.109375" style="1" bestFit="1" customWidth="1"/>
@@ -4627,7 +4627,7 @@
       <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="5.33203125" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="8" style="1" bestFit="1" customWidth="1"/>
@@ -5716,11 +5716,11 @@
   <sheetPr codeName="Sayfa4"/>
   <dimension ref="A1:G183"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="12" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9.109375" style="1" bestFit="1" customWidth="1"/>
@@ -10678,12 +10678,13 @@
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="16384" width="8.88671875" style="1"/>
+    <col min="1" max="1" width="12" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
@@ -10725,7 +10726,7 @@
       <selection activeCell="H21" sqref="H21:H22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="12" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9.109375" style="1" bestFit="1" customWidth="1"/>
@@ -14410,7 +14411,7 @@
       <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="12" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14" style="1" bestFit="1" customWidth="1"/>

</xml_diff>